<commit_message>
Added photos, finished board layout, updated readme
</commit_message>
<xml_diff>
--- a/Board/BOM.xlsx
+++ b/Board/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\TLM-18-Wrap-Up-Supervisor\Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2142BC-881D-417D-96B4-42181A009638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76B40A9-3A34-4CAC-B09E-12CD8862EEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
   <si>
     <t>Item</t>
   </si>
@@ -70,9 +70,6 @@
     <t>https://www.digikey.com/en/products/detail/nidec-copal-electronics/RE30E-1000-213-1/6469499</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/lsi-csi/LS7366R/12760871?s=N4IgjCBcoGwJxVAYygMwIYBsDOBTANCAPZQDaIALGGABxwDsIAuoQA4AuUIAyuwE4BLAHYBzEAF9CAJgqNoIFJAw4CxMiADMYBjAAMzNp0g9%2BwsZJAwN%2B%2BYuV5CJSOSo1dFDQZAcuvQaIlpMF0bZDQsBzVnTQACADUYgD8YgFYAOhT4rx9jACV0UVwAVSEBdgB5VABZXHRsAFc%2BXAlxcSA</t>
-  </si>
-  <si>
     <t>LS3766R</t>
   </si>
   <si>
@@ -128,15 +125,111 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/7447471101/3476776</t>
+  </si>
+  <si>
+    <t>Fuse Holder</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/keystone-electronics/3568/2137306</t>
+  </si>
+  <si>
+    <t>15pF Capacitor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-beyschlag-draloric-bc-components/K150J15C0GF5TL2/286457</t>
+  </si>
+  <si>
+    <t>K150J15C0GF5TL2</t>
+  </si>
+  <si>
+    <t>Power Connector</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/on-shore-technology-inc/OSTVN02A150/1588862</t>
+  </si>
+  <si>
+    <t>OSTVN02A150</t>
+  </si>
+  <si>
+    <t>DB-9 Male</t>
+  </si>
+  <si>
+    <t>DB-9 Female</t>
+  </si>
+  <si>
+    <t>A-DS 09 PP/Z-BK</t>
+  </si>
+  <si>
+    <t>A-DF 09 PP/Z-BK</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/assmann-wsw-components/A-DS-09-PP-Z-BK/10668847</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/assmann-wsw-components/A-DF-09-PP-Z-BK/10668849</t>
+  </si>
+  <si>
+    <t>Total Price</t>
+  </si>
+  <si>
+    <t>DB-9 Connector Assortment</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/ANMBEST-Connector-Terminal-Breakout-Assortment/dp/B09698YCTZ/?th=1</t>
+  </si>
+  <si>
+    <t>Items for Mechanical Assembly</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/lsi-csi/LS7366R/12760871</t>
+  </si>
+  <si>
+    <t>Items for 1 PCB</t>
+  </si>
+  <si>
+    <t>Isolated USB RS422 Interface</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/DSD-TECH-SH-U11F-Industrial-Application/dp/B083XSG1RG/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -151,7 +244,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -159,14 +252,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -445,285 +585,445 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="89.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="127.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
+        <v>6.62</v>
+      </c>
+      <c r="F3" s="5">
+        <f t="shared" ref="F3:F18" si="0">D3*E3</f>
+        <v>6.62</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>4.33</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" si="0"/>
+        <v>4.33</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.82</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" si="0"/>
+        <v>0.82</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
+        <v>6.12</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" si="0"/>
+        <v>6.12</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.39</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="0"/>
+        <v>0.39</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.92</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="0"/>
+        <v>1.84</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="8">
+        <v>7447471101</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>2.54</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="0"/>
+        <v>2.54</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="8">
+        <v>3568</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1.33</v>
+      </c>
+      <c r="F10" s="5">
+        <f t="shared" si="0"/>
+        <v>1.33</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.96</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="0"/>
+        <v>0.96</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0.71</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.71</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5">
+        <v>16.989999999999998</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="0"/>
+        <v>16.989999999999998</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B17" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
+      <c r="C17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5">
         <v>96.21</v>
       </c>
-      <c r="F2">
-        <f>D2*E2</f>
+      <c r="F17" s="5">
+        <f>D17*E17</f>
         <v>96.21</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G17" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>6.62</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F17" si="0">D3*E3</f>
-        <v>6.62</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>4.33</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>4.33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0.82</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>0.82</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>6.12</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>6.12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0.39</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>0.39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>0.92</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>1.84</v>
-      </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9">
-        <v>7447471101</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>2.54</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>2.54</v>
-      </c>
-      <c r="G9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="10">
+        <v>1</v>
+      </c>
+      <c r="E18" s="11">
+        <v>20.99</v>
+      </c>
+      <c r="F18" s="11">
+        <f>D18*E18</f>
+        <v>20.99</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="6">
+        <f>SUM(F3:F14,F16:F18)</f>
+        <v>160.65</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A15:G15"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G8" r:id="rId1" xr:uid="{32E2DC0B-C0F1-40B6-B53A-F248F046465F}"/>
+    <hyperlink ref="G12" r:id="rId2" xr:uid="{2F2A08A2-C86B-4C41-9CD9-731FA1FD1A83}"/>
+    <hyperlink ref="G3" r:id="rId3" xr:uid="{1EFA8B48-2E8C-430C-9D4E-E947169FB885}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>